<commit_message>
testes com validação cruzada
</commit_message>
<xml_diff>
--- a/resultados/Tabela_Resultados_Teste.xlsx
+++ b/resultados/Tabela_Resultados_Teste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Documents\NotebooksMateriais\previsao_custo_salario_cestas\resultados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DDAD14-7501-4113-963F-F79C1FD451A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EB7867-26C1-4DD0-A487-142DEA4AD50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BD8870E6-5BAF-48E2-97AA-8D70593EEDB5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
   <si>
     <t>RNN</t>
   </si>
@@ -60,49 +60,10 @@
     <t>Ilhéus</t>
   </si>
   <si>
-    <t>RMSE</t>
-  </si>
-  <si>
-    <t>0.02885</t>
-  </si>
-  <si>
-    <t>0.04154</t>
-  </si>
-  <si>
-    <t>0.03652</t>
-  </si>
-  <si>
-    <t>0.03856</t>
-  </si>
-  <si>
-    <t>0.02952</t>
-  </si>
-  <si>
-    <t>0.03101</t>
-  </si>
-  <si>
-    <t>Últimos 6 Meses</t>
-  </si>
-  <si>
-    <t>Conjunto de Teste</t>
-  </si>
-  <si>
-    <t>0.05263</t>
-  </si>
-  <si>
-    <t>0.06162</t>
-  </si>
-  <si>
-    <t>0.05739</t>
-  </si>
-  <si>
-    <t>0.02958</t>
-  </si>
-  <si>
-    <t>0.03838</t>
-  </si>
-  <si>
-    <t>0.06071</t>
+    <t>Últimos 3 Meses (Última Amostra)</t>
+  </si>
+  <si>
+    <t>Conjunto de Teste (36 Amostras)</t>
   </si>
 </sst>
 </file>
@@ -218,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -242,20 +203,24 @@
     <xf numFmtId="3" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -571,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF55CDF-0037-4B24-8840-D4386B0BDF82}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D17" sqref="D17:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,114 +555,92 @@
     <col min="12" max="12" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="4">
-        <v>6427</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
+        <v>6392</v>
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="4">
-        <v>8653</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
+        <v>5526</v>
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="6">
-        <v>5771</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>9</v>
+        <v>7128</v>
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
       <c r="B6" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="6">
-        <v>8471</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>12</v>
+        <v>5453</v>
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="8">
-        <v>6076</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>13</v>
+        <v>6232</v>
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
       <c r="B8" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="8">
-        <v>8023</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>11</v>
+        <v>5268</v>
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -705,123 +648,121 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="9" t="s">
         <v>1</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>8</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="4">
-        <v>13924</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
+        <v>6734</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
       <c r="B13" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="4">
-        <v>11869</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+        <v>2075</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="6">
-        <v>13866</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
+        <v>7015</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
       <c r="B15" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="6">
-        <v>8619</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="8">
-        <v>13097</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+        <v>6872</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
       <c r="B17" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="8">
-        <v>6574</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>20</v>
+        <v>1207</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="10"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -829,7 +770,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -837,7 +778,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -845,7 +786,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -853,7 +794,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -861,7 +802,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -869,7 +810,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -877,7 +818,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -885,7 +826,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -893,19 +834,19 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -913,11 +854,11 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A10:C10"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:D10"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>

</xml_diff>